<commit_message>
Update tracker with vax 2 and clean up results
</commit_message>
<xml_diff>
--- a/data/clinical/Participant Tracker.xlsx
+++ b/data/clinical/Participant Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlesgleason/Documents/GitHub/reshaping-pod-b/data/clinical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1B4B14-2A13-774F-A232-C272412F6BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFD6463-E621-274F-9FCE-18DFDA7A8E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2700" yWindow="2820" windowWidth="26440" windowHeight="15440" xr2:uid="{D4A80C08-9BAA-D746-8412-0704219F9B1E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="32">
   <si>
     <t>Participant ID</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Sex</t>
   </si>
   <si>
-    <t>Vaccine Date</t>
-  </si>
-  <si>
     <t>Infection Pre-Vaccine?</t>
   </si>
   <si>
@@ -129,16 +126,29 @@
   </si>
   <si>
     <t>Moderna</t>
+  </si>
+  <si>
+    <t>Vaccine Date 1</t>
+  </si>
+  <si>
+    <t>Vaccine Date 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -164,10 +174,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,9 +494,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C6B0FB-A248-A44A-A65B-B1EA088DAF97}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -492,11 +506,12 @@
     <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,20 +521,23 @@
       <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -527,23 +545,26 @@
         <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1">
         <v>46741</v>
       </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="E2" s="3">
+        <v>46761</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1">
         <v>46421</v>
       </c>
-      <c r="G2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -551,22 +572,25 @@
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1">
         <v>46753</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3">
+        <v>46778</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -574,22 +598,25 @@
         <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1">
         <v>46722</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3">
+        <v>46747</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -597,22 +624,25 @@
         <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1">
         <v>46754</v>
       </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="E5" s="3">
+        <v>46774</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="1">
         <v>46449</v>
       </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -620,22 +650,25 @@
         <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1">
         <v>46710</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3">
+        <v>46732</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -643,22 +676,25 @@
         <v>63</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1">
         <v>46722</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3">
+        <v>46745</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -666,22 +702,25 @@
         <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1">
         <v>46768</v>
       </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="E8" s="3">
+        <v>46790</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="1">
         <v>46450</v>
       </c>
-      <c r="G8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -689,22 +728,25 @@
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1">
         <v>46705</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3">
+        <v>46727</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -712,22 +754,25 @@
         <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1">
         <v>46758</v>
       </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="E10" s="3">
+        <v>46779</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="1">
         <v>46475</v>
       </c>
-      <c r="G10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -735,22 +780,25 @@
         <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1">
         <v>46755</v>
       </c>
-      <c r="E11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="E11" s="3">
+        <v>46774</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="1">
         <v>46394</v>
       </c>
-      <c r="G11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -758,22 +806,25 @@
         <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1">
         <v>46752</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3">
+        <v>46774</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -781,22 +832,25 @@
         <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1">
         <v>46767</v>
       </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="1">
+      <c r="E13" s="3">
+        <v>46786</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="1">
         <v>46454</v>
       </c>
-      <c r="G13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -804,22 +858,25 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1">
         <v>46762</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3">
+        <v>46790</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -827,22 +884,25 @@
         <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="1">
         <v>46733</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="3">
+        <v>46756</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -850,22 +910,25 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="1">
         <v>46795</v>
       </c>
-      <c r="E16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="1">
+      <c r="E16" s="3">
+        <v>46815</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="1">
         <v>46475</v>
       </c>
-      <c r="G16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -873,22 +936,25 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="1">
         <v>46755</v>
       </c>
-      <c r="E17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="1">
+      <c r="E17" s="3">
+        <v>46775</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="1">
         <v>46314</v>
       </c>
-      <c r="G17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -896,19 +962,22 @@
         <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1">
         <v>46763</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="3">
+        <v>46791</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" t="s">
-        <v>30</v>
+      <c r="H18" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>